<commit_message>
subir los cambios de juego
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2275,6 +2275,381 @@
         <v>30200</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-02-22 11:35:05</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L25" t="n">
+        <v>100</v>
+      </c>
+      <c r="M25" t="n">
+        <v>500</v>
+      </c>
+      <c r="N25" t="n">
+        <v>10</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5</v>
+      </c>
+      <c r="P25" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>500</v>
+      </c>
+      <c r="R25" t="n">
+        <v>7</v>
+      </c>
+      <c r="S25" t="n">
+        <v>3</v>
+      </c>
+      <c r="T25" t="n">
+        <v>100</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1</v>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Data/bombayauto.xlsx</t>
+        </is>
+      </c>
+      <c r="W25" t="n">
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2024-02-24 00:03:34</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L26" t="n">
+        <v>100</v>
+      </c>
+      <c r="M26" t="n">
+        <v>500</v>
+      </c>
+      <c r="N26" t="n">
+        <v>10</v>
+      </c>
+      <c r="O26" t="n">
+        <v>5</v>
+      </c>
+      <c r="P26" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>200</v>
+      </c>
+      <c r="R26" t="n">
+        <v>8</v>
+      </c>
+      <c r="S26" t="n">
+        <v>3</v>
+      </c>
+      <c r="T26" t="n">
+        <v>100</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1</v>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Data/bombayauto.xlsx</t>
+        </is>
+      </c>
+      <c r="W26" t="n">
+        <v>-30800</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2024-02-24 00:20:11</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L27" t="n">
+        <v>100</v>
+      </c>
+      <c r="M27" t="n">
+        <v>500</v>
+      </c>
+      <c r="N27" t="n">
+        <v>10</v>
+      </c>
+      <c r="O27" t="n">
+        <v>5</v>
+      </c>
+      <c r="P27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>500</v>
+      </c>
+      <c r="R27" t="n">
+        <v>8</v>
+      </c>
+      <c r="S27" t="n">
+        <v>3</v>
+      </c>
+      <c r="T27" t="n">
+        <v>100</v>
+      </c>
+      <c r="U27" t="n">
+        <v>1</v>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Data/bombayauto.xlsx</t>
+        </is>
+      </c>
+      <c r="W27" t="n">
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-02-24 01:22:17</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>43</v>
+      </c>
+      <c r="C28" t="n">
+        <v>29</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" t="n">
+        <v>12</v>
+      </c>
+      <c r="F28" t="n">
+        <v>14</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L28" t="n">
+        <v>100</v>
+      </c>
+      <c r="M28" t="n">
+        <v>500</v>
+      </c>
+      <c r="N28" t="n">
+        <v>10</v>
+      </c>
+      <c r="O28" t="n">
+        <v>5</v>
+      </c>
+      <c r="P28" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>200</v>
+      </c>
+      <c r="R28" t="n">
+        <v>8</v>
+      </c>
+      <c r="S28" t="n">
+        <v>3</v>
+      </c>
+      <c r="T28" t="n">
+        <v>80</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.6744186046511628</v>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W28" t="n">
+        <v>-160200</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-02-24 13:52:25</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>14</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L29" t="n">
+        <v>100</v>
+      </c>
+      <c r="M29" t="n">
+        <v>500</v>
+      </c>
+      <c r="N29" t="n">
+        <v>10</v>
+      </c>
+      <c r="O29" t="n">
+        <v>5</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>200</v>
+      </c>
+      <c r="R29" t="n">
+        <v>8</v>
+      </c>
+      <c r="S29" t="n">
+        <v>3</v>
+      </c>
+      <c r="T29" t="n">
+        <v>70</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Data/bombayauto.xlsx</t>
+        </is>
+      </c>
+      <c r="W29" t="n">
+        <v>43800</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios de array a dicionario en simulacion
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3025,6 +3025,81 @@
         <v>1161000</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024-03-29 02:10:45</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>31</v>
+      </c>
+      <c r="C35" t="n">
+        <v>11</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>5</v>
+      </c>
+      <c r="F35" t="n">
+        <v>6</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L35" t="n">
+        <v>100</v>
+      </c>
+      <c r="M35" t="n">
+        <v>500</v>
+      </c>
+      <c r="N35" t="n">
+        <v>10</v>
+      </c>
+      <c r="O35" t="n">
+        <v>9</v>
+      </c>
+      <c r="P35" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>200</v>
+      </c>
+      <c r="R35" t="n">
+        <v>3</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1</v>
+      </c>
+      <c r="T35" t="n">
+        <v>70</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.3548387096774194</v>
+      </c>
+      <c r="V35" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W35" t="n">
+        <v>-32600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
enviar cambios de optimizacion
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +549,11 @@
           <t>Ganancia</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Juego</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -624,6 +629,7 @@
       <c r="W2" t="n">
         <v>273000</v>
       </c>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -699,6 +705,7 @@
       <c r="W3" t="n">
         <v>279000</v>
       </c>
+      <c r="X3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -774,6 +781,7 @@
       <c r="W4" t="n">
         <v>-228000</v>
       </c>
+      <c r="X4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -849,6 +857,7 @@
       <c r="W5" t="n">
         <v>-162000</v>
       </c>
+      <c r="X5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -924,6 +933,7 @@
       <c r="W6" t="n">
         <v>309000</v>
       </c>
+      <c r="X6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -999,6 +1009,7 @@
       <c r="W7" t="n">
         <v>75000</v>
       </c>
+      <c r="X7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1074,6 +1085,7 @@
       <c r="W8" t="n">
         <v>-72000</v>
       </c>
+      <c r="X8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1149,6 +1161,7 @@
       <c r="W9" t="n">
         <v>410000</v>
       </c>
+      <c r="X9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1224,6 +1237,7 @@
       <c r="W10" t="n">
         <v>-25600</v>
       </c>
+      <c r="X10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1299,6 +1313,7 @@
       <c r="W11" t="n">
         <v>244000</v>
       </c>
+      <c r="X11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1374,6 +1389,7 @@
       <c r="W12" t="n">
         <v>299000</v>
       </c>
+      <c r="X12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1449,6 +1465,7 @@
       <c r="W13" t="n">
         <v>-667000</v>
       </c>
+      <c r="X13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1524,6 +1541,7 @@
       <c r="W14" t="n">
         <v>229500</v>
       </c>
+      <c r="X14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1599,6 +1617,7 @@
       <c r="W15" t="n">
         <v>255000</v>
       </c>
+      <c r="X15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1674,6 +1693,7 @@
       <c r="W16" t="n">
         <v>1581000</v>
       </c>
+      <c r="X16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1749,6 +1769,7 @@
       <c r="W17" t="n">
         <v>-21600</v>
       </c>
+      <c r="X17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1824,6 +1845,7 @@
       <c r="W18" t="n">
         <v>148000</v>
       </c>
+      <c r="X18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1899,6 +1921,7 @@
       <c r="W19" t="n">
         <v>510000</v>
       </c>
+      <c r="X19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1974,6 +1997,7 @@
       <c r="W20" t="n">
         <v>52500</v>
       </c>
+      <c r="X20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2049,6 +2073,7 @@
       <c r="W21" t="n">
         <v>-111000</v>
       </c>
+      <c r="X21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2124,6 +2149,7 @@
       <c r="W22" t="n">
         <v>-53800</v>
       </c>
+      <c r="X22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2199,6 +2225,7 @@
       <c r="W23" t="n">
         <v>-67600</v>
       </c>
+      <c r="X23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2274,6 +2301,7 @@
       <c r="W24" t="n">
         <v>30200</v>
       </c>
+      <c r="X24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2349,6 +2377,7 @@
       <c r="W25" t="n">
         <v>98000</v>
       </c>
+      <c r="X25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2424,6 +2453,7 @@
       <c r="W26" t="n">
         <v>-30800</v>
       </c>
+      <c r="X26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2499,6 +2529,7 @@
       <c r="W27" t="n">
         <v>53000</v>
       </c>
+      <c r="X27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2574,6 +2605,7 @@
       <c r="W28" t="n">
         <v>-160200</v>
       </c>
+      <c r="X28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2649,6 +2681,7 @@
       <c r="W29" t="n">
         <v>43800</v>
       </c>
+      <c r="X29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2724,6 +2757,7 @@
       <c r="W30" t="n">
         <v>-18600</v>
       </c>
+      <c r="X30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2799,6 +2833,7 @@
       <c r="W31" t="n">
         <v>-488000</v>
       </c>
+      <c r="X31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2874,6 +2909,7 @@
       <c r="W32" t="n">
         <v>392000</v>
       </c>
+      <c r="X32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2949,6 +2985,7 @@
       <c r="W33" t="n">
         <v>0</v>
       </c>
+      <c r="X33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3024,6 +3061,7 @@
       <c r="W34" t="n">
         <v>1161000</v>
       </c>
+      <c r="X34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3098,6 +3136,87 @@
       </c>
       <c r="W35" t="n">
         <v>-32600</v>
+      </c>
+      <c r="X35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2024-03-30 19:24:12</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L36" t="n">
+        <v>100</v>
+      </c>
+      <c r="M36" t="n">
+        <v>500</v>
+      </c>
+      <c r="N36" t="n">
+        <v>10</v>
+      </c>
+      <c r="O36" t="n">
+        <v>9</v>
+      </c>
+      <c r="P36" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R36" t="n">
+        <v>3</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1</v>
+      </c>
+      <c r="T36" t="n">
+        <v>100</v>
+      </c>
+      <c r="U36" t="n">
+        <v>1</v>
+      </c>
+      <c r="V36" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W36" t="n">
+        <v>29000</v>
+      </c>
+      <c r="X36" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en la en los nombres y demas
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3219,6 +3219,486 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2024-04-07 00:23:03</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L37" t="n">
+        <v>100</v>
+      </c>
+      <c r="M37" t="n">
+        <v>500</v>
+      </c>
+      <c r="N37" t="n">
+        <v>10</v>
+      </c>
+      <c r="O37" t="n">
+        <v>9</v>
+      </c>
+      <c r="P37" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R37" t="n">
+        <v>5</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T37" t="n">
+        <v>100</v>
+      </c>
+      <c r="U37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W37" t="n">
+        <v>196000</v>
+      </c>
+      <c r="X37" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2024-04-14 19:49:46</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L38" t="n">
+        <v>100</v>
+      </c>
+      <c r="M38" t="n">
+        <v>500</v>
+      </c>
+      <c r="N38" t="n">
+        <v>10</v>
+      </c>
+      <c r="O38" t="n">
+        <v>9</v>
+      </c>
+      <c r="P38" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R38" t="n">
+        <v>5</v>
+      </c>
+      <c r="S38" t="n">
+        <v>1</v>
+      </c>
+      <c r="T38" t="n">
+        <v>100</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1</v>
+      </c>
+      <c r="V38" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W38" t="n">
+        <v>136000</v>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2024-04-18 21:37:03</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>23</v>
+      </c>
+      <c r="C39" t="n">
+        <v>16</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" t="n">
+        <v>7</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L39" t="n">
+        <v>100</v>
+      </c>
+      <c r="M39" t="n">
+        <v>500</v>
+      </c>
+      <c r="N39" t="n">
+        <v>10</v>
+      </c>
+      <c r="O39" t="n">
+        <v>9</v>
+      </c>
+      <c r="P39" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>500</v>
+      </c>
+      <c r="R39" t="n">
+        <v>5</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1</v>
+      </c>
+      <c r="T39" t="n">
+        <v>90</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.6956521739130435</v>
+      </c>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W39" t="n">
+        <v>-314500</v>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2024-04-20 22:25:44</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>188</v>
+      </c>
+      <c r="C40" t="n">
+        <v>34</v>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>13</v>
+      </c>
+      <c r="F40" t="n">
+        <v>17</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L40" t="n">
+        <v>100</v>
+      </c>
+      <c r="M40" t="n">
+        <v>500</v>
+      </c>
+      <c r="N40" t="n">
+        <v>10</v>
+      </c>
+      <c r="O40" t="n">
+        <v>9</v>
+      </c>
+      <c r="P40" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>500</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>10</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.1808510638297872</v>
+      </c>
+      <c r="V40" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W40" t="n">
+        <v>59500</v>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-04-20 23:11:48</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>67</v>
+      </c>
+      <c r="C41" t="n">
+        <v>8</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L41" t="n">
+        <v>100</v>
+      </c>
+      <c r="M41" t="n">
+        <v>500</v>
+      </c>
+      <c r="N41" t="n">
+        <v>10</v>
+      </c>
+      <c r="O41" t="n">
+        <v>9</v>
+      </c>
+      <c r="P41" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>500</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>50</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.1194029850746269</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W41" t="n">
+        <v>-41000</v>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-04-21 01:04:36</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>14</v>
+      </c>
+      <c r="C42" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="n">
+        <v>6</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L42" t="n">
+        <v>100</v>
+      </c>
+      <c r="M42" t="n">
+        <v>500</v>
+      </c>
+      <c r="N42" t="n">
+        <v>10</v>
+      </c>
+      <c r="O42" t="n">
+        <v>9</v>
+      </c>
+      <c r="P42" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R42" t="n">
+        <v>3</v>
+      </c>
+      <c r="S42" t="n">
+        <v>1</v>
+      </c>
+      <c r="T42" t="n">
+        <v>90</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W42" t="n">
+        <v>533000</v>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
nuevos jugos arreglo la consulta de probabiliad cambiar los juegos a lightinh para obtener esa base
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3699,6 +3699,566 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-04-27 18:43:58</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>77</v>
+      </c>
+      <c r="C43" t="n">
+        <v>26</v>
+      </c>
+      <c r="D43" t="n">
+        <v>6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>10</v>
+      </c>
+      <c r="F43" t="n">
+        <v>10</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L43" t="n">
+        <v>100</v>
+      </c>
+      <c r="M43" t="n">
+        <v>500</v>
+      </c>
+      <c r="N43" t="n">
+        <v>10</v>
+      </c>
+      <c r="O43" t="n">
+        <v>9</v>
+      </c>
+      <c r="P43" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>500</v>
+      </c>
+      <c r="R43" t="n">
+        <v>3</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1</v>
+      </c>
+      <c r="T43" t="n">
+        <v>20</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0.3376623376623377</v>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W43" t="n">
+        <v>-206500</v>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-04-27 18:59:38</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>61</v>
+      </c>
+      <c r="C44" t="n">
+        <v>51</v>
+      </c>
+      <c r="D44" t="n">
+        <v>14</v>
+      </c>
+      <c r="E44" t="n">
+        <v>37</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L44" t="n">
+        <v>100</v>
+      </c>
+      <c r="M44" t="n">
+        <v>500</v>
+      </c>
+      <c r="N44" t="n">
+        <v>10</v>
+      </c>
+      <c r="O44" t="n">
+        <v>9</v>
+      </c>
+      <c r="P44" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>200</v>
+      </c>
+      <c r="R44" t="n">
+        <v>20</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
+      <c r="T44" t="n">
+        <v>50</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0.8360655737704918</v>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W44" t="n">
+        <v>517800</v>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-04-27 20:05:10</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>23</v>
+      </c>
+      <c r="C45" t="n">
+        <v>22</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" t="n">
+        <v>9</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L45" t="n">
+        <v>100</v>
+      </c>
+      <c r="M45" t="n">
+        <v>500</v>
+      </c>
+      <c r="N45" t="n">
+        <v>10</v>
+      </c>
+      <c r="O45" t="n">
+        <v>9</v>
+      </c>
+      <c r="P45" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>200</v>
+      </c>
+      <c r="R45" t="n">
+        <v>10</v>
+      </c>
+      <c r="S45" t="n">
+        <v>1</v>
+      </c>
+      <c r="T45" t="n">
+        <v>90</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W45" t="n">
+        <v>161000</v>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-04-27 20:46:17</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>16</v>
+      </c>
+      <c r="C46" t="n">
+        <v>14</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L46" t="n">
+        <v>100</v>
+      </c>
+      <c r="M46" t="n">
+        <v>500</v>
+      </c>
+      <c r="N46" t="n">
+        <v>10</v>
+      </c>
+      <c r="O46" t="n">
+        <v>9</v>
+      </c>
+      <c r="P46" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>500</v>
+      </c>
+      <c r="R46" t="n">
+        <v>10</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T46" t="n">
+        <v>90</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W46" t="n">
+        <v>-376000</v>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-04-28 00:07:12</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>13</v>
+      </c>
+      <c r="C47" t="n">
+        <v>11</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4</v>
+      </c>
+      <c r="F47" t="n">
+        <v>4</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L47" t="n">
+        <v>100</v>
+      </c>
+      <c r="M47" t="n">
+        <v>500</v>
+      </c>
+      <c r="N47" t="n">
+        <v>10</v>
+      </c>
+      <c r="O47" t="n">
+        <v>9</v>
+      </c>
+      <c r="P47" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R47" t="n">
+        <v>5</v>
+      </c>
+      <c r="S47" t="n">
+        <v>1</v>
+      </c>
+      <c r="T47" t="n">
+        <v>90</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W47" t="n">
+        <v>230000</v>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-04-28 18:36:21</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>16</v>
+      </c>
+      <c r="C48" t="n">
+        <v>11</v>
+      </c>
+      <c r="D48" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L48" t="n">
+        <v>100</v>
+      </c>
+      <c r="M48" t="n">
+        <v>500</v>
+      </c>
+      <c r="N48" t="n">
+        <v>10</v>
+      </c>
+      <c r="O48" t="n">
+        <v>9</v>
+      </c>
+      <c r="P48" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>100</v>
+      </c>
+      <c r="R48" t="n">
+        <v>5</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1</v>
+      </c>
+      <c r="T48" t="n">
+        <v>90</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W48" t="n">
+        <v>-9200</v>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-04-29 00:32:25</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>12</v>
+      </c>
+      <c r="C49" t="n">
+        <v>10</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4</v>
+      </c>
+      <c r="F49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L49" t="n">
+        <v>100</v>
+      </c>
+      <c r="M49" t="n">
+        <v>500</v>
+      </c>
+      <c r="N49" t="n">
+        <v>10</v>
+      </c>
+      <c r="O49" t="n">
+        <v>9</v>
+      </c>
+      <c r="P49" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>200</v>
+      </c>
+      <c r="R49" t="n">
+        <v>5</v>
+      </c>
+      <c r="S49" t="n">
+        <v>1</v>
+      </c>
+      <c r="T49" t="n">
+        <v>90</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W49" t="n">
+        <v>15000</v>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
CONFIMAR LOS CAMBIOS DE GRU
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X53"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4579,6 +4579,486 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-05-04 21:08:45</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>12</v>
+      </c>
+      <c r="C54" t="n">
+        <v>8</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L54" t="n">
+        <v>100</v>
+      </c>
+      <c r="M54" t="n">
+        <v>500</v>
+      </c>
+      <c r="N54" t="n">
+        <v>10</v>
+      </c>
+      <c r="O54" t="n">
+        <v>9</v>
+      </c>
+      <c r="P54" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>400</v>
+      </c>
+      <c r="R54" t="n">
+        <v>5</v>
+      </c>
+      <c r="S54" t="n">
+        <v>1</v>
+      </c>
+      <c r="T54" t="n">
+        <v>90</v>
+      </c>
+      <c r="U54" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W54" t="n">
+        <v>-41200</v>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-05-04 23:16:28</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>14</v>
+      </c>
+      <c r="C55" t="n">
+        <v>9</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L55" t="n">
+        <v>100</v>
+      </c>
+      <c r="M55" t="n">
+        <v>500</v>
+      </c>
+      <c r="N55" t="n">
+        <v>10</v>
+      </c>
+      <c r="O55" t="n">
+        <v>9</v>
+      </c>
+      <c r="P55" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>100</v>
+      </c>
+      <c r="R55" t="n">
+        <v>5</v>
+      </c>
+      <c r="S55" t="n">
+        <v>1</v>
+      </c>
+      <c r="T55" t="n">
+        <v>90</v>
+      </c>
+      <c r="U55" t="n">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W55" t="n">
+        <v>-23900</v>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-05-06 21:50:51</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>9</v>
+      </c>
+      <c r="C56" t="n">
+        <v>5</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L56" t="n">
+        <v>100</v>
+      </c>
+      <c r="M56" t="n">
+        <v>500</v>
+      </c>
+      <c r="N56" t="n">
+        <v>10</v>
+      </c>
+      <c r="O56" t="n">
+        <v>9</v>
+      </c>
+      <c r="P56" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>100</v>
+      </c>
+      <c r="R56" t="n">
+        <v>5</v>
+      </c>
+      <c r="S56" t="n">
+        <v>1</v>
+      </c>
+      <c r="T56" t="n">
+        <v>90</v>
+      </c>
+      <c r="U56" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W56" t="n">
+        <v>-45300</v>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-05-09 23:17:23</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>10</v>
+      </c>
+      <c r="C57" t="n">
+        <v>6</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>4</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L57" t="n">
+        <v>100</v>
+      </c>
+      <c r="M57" t="n">
+        <v>500</v>
+      </c>
+      <c r="N57" t="n">
+        <v>10</v>
+      </c>
+      <c r="O57" t="n">
+        <v>9</v>
+      </c>
+      <c r="P57" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>400</v>
+      </c>
+      <c r="R57" t="n">
+        <v>5</v>
+      </c>
+      <c r="S57" t="n">
+        <v>1</v>
+      </c>
+      <c r="T57" t="n">
+        <v>90</v>
+      </c>
+      <c r="U57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W57" t="n">
+        <v>-73200</v>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-05-14 00:10:08</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>7</v>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3</v>
+      </c>
+      <c r="G58" t="n">
+        <v>2</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L58" t="n">
+        <v>100</v>
+      </c>
+      <c r="M58" t="n">
+        <v>500</v>
+      </c>
+      <c r="N58" t="n">
+        <v>10</v>
+      </c>
+      <c r="O58" t="n">
+        <v>9</v>
+      </c>
+      <c r="P58" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>400</v>
+      </c>
+      <c r="R58" t="n">
+        <v>5</v>
+      </c>
+      <c r="S58" t="n">
+        <v>1</v>
+      </c>
+      <c r="T58" t="n">
+        <v>90</v>
+      </c>
+      <c r="U58" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W58" t="n">
+        <v>47200</v>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-05-26 01:14:41</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>9</v>
+      </c>
+      <c r="C59" t="n">
+        <v>7</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L59" t="n">
+        <v>100</v>
+      </c>
+      <c r="M59" t="n">
+        <v>500</v>
+      </c>
+      <c r="N59" t="n">
+        <v>10</v>
+      </c>
+      <c r="O59" t="n">
+        <v>9</v>
+      </c>
+      <c r="P59" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R59" t="n">
+        <v>5</v>
+      </c>
+      <c r="S59" t="n">
+        <v>1</v>
+      </c>
+      <c r="T59" t="n">
+        <v>90</v>
+      </c>
+      <c r="U59" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W59" t="n">
+        <v>54000</v>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en el resultados y busqueda de parametros
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:X63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5059,6 +5059,326 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-06-06 18:52:18</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>39</v>
+      </c>
+      <c r="C60" t="n">
+        <v>28</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" t="n">
+        <v>10</v>
+      </c>
+      <c r="F60" t="n">
+        <v>4</v>
+      </c>
+      <c r="G60" t="n">
+        <v>11</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L60" t="n">
+        <v>100</v>
+      </c>
+      <c r="M60" t="n">
+        <v>500</v>
+      </c>
+      <c r="N60" t="n">
+        <v>10</v>
+      </c>
+      <c r="O60" t="n">
+        <v>9</v>
+      </c>
+      <c r="P60" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R60" t="n">
+        <v>5</v>
+      </c>
+      <c r="S60" t="n">
+        <v>2</v>
+      </c>
+      <c r="T60" t="n">
+        <v>70</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0.717948717948718</v>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W60" t="n">
+        <v>-103000</v>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-06-06 23:24:27</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>39</v>
+      </c>
+      <c r="C61" t="n">
+        <v>29</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" t="n">
+        <v>15</v>
+      </c>
+      <c r="F61" t="n">
+        <v>6</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L61" t="n">
+        <v>100</v>
+      </c>
+      <c r="M61" t="n">
+        <v>500</v>
+      </c>
+      <c r="N61" t="n">
+        <v>10</v>
+      </c>
+      <c r="O61" t="n">
+        <v>9</v>
+      </c>
+      <c r="P61" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R61" t="n">
+        <v>5</v>
+      </c>
+      <c r="S61" t="n">
+        <v>2</v>
+      </c>
+      <c r="T61" t="n">
+        <v>70</v>
+      </c>
+      <c r="U61" t="n">
+        <v>0.7435897435897436</v>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W61" t="n">
+        <v>-29000</v>
+      </c>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-06-10 22:38:38</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>14</v>
+      </c>
+      <c r="C62" t="n">
+        <v>10</v>
+      </c>
+      <c r="D62" t="n">
+        <v>4</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L62" t="n">
+        <v>100</v>
+      </c>
+      <c r="M62" t="n">
+        <v>500</v>
+      </c>
+      <c r="N62" t="n">
+        <v>10</v>
+      </c>
+      <c r="O62" t="n">
+        <v>9</v>
+      </c>
+      <c r="P62" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R62" t="n">
+        <v>5</v>
+      </c>
+      <c r="S62" t="n">
+        <v>2</v>
+      </c>
+      <c r="T62" t="n">
+        <v>70</v>
+      </c>
+      <c r="U62" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W62" t="n">
+        <v>150000</v>
+      </c>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-06-13 19:36:58</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>35</v>
+      </c>
+      <c r="C63" t="n">
+        <v>21</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="n">
+        <v>5</v>
+      </c>
+      <c r="F63" t="n">
+        <v>5</v>
+      </c>
+      <c r="G63" t="n">
+        <v>9</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L63" t="n">
+        <v>100</v>
+      </c>
+      <c r="M63" t="n">
+        <v>500</v>
+      </c>
+      <c r="N63" t="n">
+        <v>10</v>
+      </c>
+      <c r="O63" t="n">
+        <v>9</v>
+      </c>
+      <c r="P63" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R63" t="n">
+        <v>5</v>
+      </c>
+      <c r="S63" t="n">
+        <v>2</v>
+      </c>
+      <c r="T63" t="n">
+        <v>70</v>
+      </c>
+      <c r="U63" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+      <c r="W63" t="n">
+        <v>-907000</v>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
arreglo muchos errores en el keras y cambios en el modelo
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,6 +635,86 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-07-22 00:05:53</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L3" t="n">
+        <v>100</v>
+      </c>
+      <c r="M3" t="n">
+        <v>500</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" t="n">
+        <v>6</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>./Data/Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>233000</v>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en los botones
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,6 +715,86 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-07-22 21:13:19</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L4" t="n">
+        <v>100</v>
+      </c>
+      <c r="M4" t="n">
+        <v>500</v>
+      </c>
+      <c r="N4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>./Data/Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W4" t="n">
+        <v>328000</v>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
colocacion de llenado automatico en gettypes de combo box de con los datos que hay
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,11 @@
           <t>Juego</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Predecidos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -634,6 +639,7 @@
           <t>No es Simulación</t>
         </is>
       </c>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -714,6 +720,7 @@
           <t>No es Simulación</t>
         </is>
       </c>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -793,6 +800,72 @@
         <is>
           <t>No es Simulación</t>
         </is>
+      </c>
+      <c r="Y4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-07-28 16:00:48</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="n">
+        <v>10</v>
+      </c>
+      <c r="O5" t="n">
+        <v>6</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>20</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>./Data/Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
si borro la carpeta pyqt5
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,6 +868,136 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-04 22:11:04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>10</v>
+      </c>
+      <c r="O6" t="n">
+        <v>6</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>20</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-04 22:13:50</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>5</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>20</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modificacion de rutas relativas
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,6 +868,201 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-08-01 15:23:05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>10</v>
+      </c>
+      <c r="O6" t="n">
+        <v>6</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
+        <v>5</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="n">
+        <v>20</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>C:\Users\jgcorrea\Desktop\Repositorio\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-08-01 15:27:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="n">
+        <v>5</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
+        <v>20</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>C:\Users\jgcorrea\Desktop\Repositorio\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-08-01 15:33:43</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>10</v>
+      </c>
+      <c r="O8" t="n">
+        <v>6</v>
+      </c>
+      <c r="P8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="n">
+        <v>5</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="n">
+        <v>20</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>C:\Users\jgcorrea\Desktop\Repositorio\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en nombres y problema de que no se borrarba las estadisticas
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1063,6 +1063,71 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-09-01 21:15:40</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="n">
+        <v>10</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6</v>
+      </c>
+      <c r="P9" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="n">
+        <v>5</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
+        <v>50</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta_ejecutable\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y9" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
colocacion de modelos nuevo con numeros anteriores
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1648,6 +1648,71 @@
         <v>56</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-09-08 20:30:11</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="n">
+        <v>10</v>
+      </c>
+      <c r="O18" t="n">
+        <v>4</v>
+      </c>
+      <c r="P18" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="n">
+        <v>3</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>50</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
se  juego un poco mas en la electromecanica
</commit_message>
<xml_diff>
--- a/Reporte_juego.xlsx
+++ b/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1713,6 +1713,136 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-10-05 14:06:44</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>7</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="n">
+        <v>10</v>
+      </c>
+      <c r="O19" t="n">
+        <v>10</v>
+      </c>
+      <c r="P19" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>5</v>
+      </c>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="n">
+        <v>50</v>
+      </c>
+      <c r="U19" t="n">
+        <v>1</v>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y19" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-10-05 14:54:13</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="n">
+        <v>10</v>
+      </c>
+      <c r="O20" t="n">
+        <v>10</v>
+      </c>
+      <c r="P20" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>5</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="n">
+        <v>20</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>